<commit_message>
Gound objects spawn bug fixed Global constants defined
</commit_message>
<xml_diff>
--- a/Assets/Levels/Level1/FuelTanks.xlsx
+++ b/Assets/Levels/Level1/FuelTanks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josip\source\repos\Space Retro Trouble\Assets\Levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josip\source\repos\Space Retro Trouble\Assets\Levels\Level1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EB5D76-597F-4F3E-BD68-68DEA5CF6397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0276C3D4-B92C-4D06-B995-013374B66420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{543AD0B1-5B18-4FA5-8003-7C9D3464DA33}"/>
   </bookViews>
@@ -83,8 +83,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Zarez" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -396,40 +396,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF369A3-DCC3-4973-AC1E-EF925DA3C8EE}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E14"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>682</v>
       </c>
       <c r="B1" s="1">
         <v>128</v>
       </c>
-      <c r="C1" s="1">
-        <v>200</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f t="shared" ref="A2:A12" si="0">+A1+62*11</f>
+        <f t="shared" ref="A2" si="0">+A1+62*11</f>
         <v>1364</v>
       </c>
       <c r="B2" s="1">
         <v>128</v>
-      </c>
-      <c r="C2" s="1">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set origin to sprite center for flying objects
</commit_message>
<xml_diff>
--- a/Assets/Levels/Level1/FuelTanks.xlsx
+++ b/Assets/Levels/Level1/FuelTanks.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josip\source\repos\Space Retro Trouble\Assets\Levels\Level1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0276C3D4-B92C-4D06-B995-013374B66420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D87241CF-4CD0-48CF-AEC9-4CFBE6B84A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{543AD0B1-5B18-4FA5-8003-7C9D3464DA33}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tiles" sheetId="1" r:id="rId1"/>
+    <sheet name="FuelTanks" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,19 +410,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>682</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1">
-        <v>128</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f t="shared" ref="A2" si="0">+A1+62*11</f>
-        <v>1364</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
-        <v>128</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>